<commit_message>
modif dossier public par www, ajout d'une possibilité de status dans les étapes de la fiche projet
</commit_message>
<xml_diff>
--- a/data/data_projets.xlsx
+++ b/data/data_projets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dim\clone_repo\portfolio\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66515715-E511-4612-9588-C46FCEEC33E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E55709-979E-4D24-9633-88CCE63B659C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="207">
   <si>
     <t>title</t>
   </si>
@@ -241,15 +241,9 @@
     <t>video_link</t>
   </si>
   <si>
-    <t>Dans le cadre de l'analyse détaillée des performances lors de championnats sportifs, notamment en judo, l'identification et l'analyse précises des techniques utilisées par les athlètes constituent un réel défi. Ce projet répond au besoin de suivre précisément les mouvements des judokas afin de permettre une analyse statistique approfondie des techniques utilisées et de la performance globale.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Fournir une solution automatisée capable d'analyser des combats de judo en temps réel, facilitant ainsi la collecte de statistiques et l'évaluation des performances.</t>
   </si>
   <si>
-    <t>Détection et suivi précis des individus avec estimation de leurs poses pour une analyse détaillée des mouvements.</t>
-  </si>
-  <si>
     <t>Vidéo</t>
   </si>
   <si>
@@ -265,15 +259,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>Obtention d'une vidéo annotée permettant de visualiser clairement les positions et les mouvements des judokas.|-|Possibilité d'une analyse statistique poussée sur les techniques utilisées et la performance individuelle des athlètes.|-|Impact métier majeur : Optimisation des entraînements et stratégie en compétition basée sur des données précises et exploitables.</t>
-  </si>
-  <si>
-    <t>Défis techniques liés à la précision de détection des poses en cas de mouvements rapides.|-|Ajustement fin des paramètres du tracker (DeepSORT) pour une performance optimale.|-|Importance de choisir des modèles adaptés aux spécificités des mouvements sportifs rapides.</t>
-  </si>
-  <si>
-    <t>Intégration d'un mécanisme dynamique d'ajustement automatique du nombre maximal de poses détectées.|-|Optimisation de la vitesse de traitement pour une analyse en temps réel améliorée.|-|Exploration de techniques avancées d'apprentissage profond pour améliorer la précision des détections.</t>
-  </si>
-  <si>
     <t>judo_tracking.webm</t>
   </si>
   <si>
@@ -609,17 +594,6 @@
 GitHub pour le versionnement</t>
   </si>
   <si>
-    <t>Collecte et extraction des données IMDB et TMDB.
-|-|
-Nettoyage, jointures et exploration approfondie des données.
-|-|
-Identification des caractéristiques importantes pour le modèle.
-|-|
-Développement et entraînement d'un modèle de recommandation basé sur le machine learning.
-|-|
-Création d’une interface interactive avec Streamlit pour afficher les recommandations et les KPI associés.</t>
-  </si>
-  <si>
     <t>flixoucreuse_results.webp</t>
   </si>
   <si>
@@ -730,6 +704,89 @@
 Docker pour la conteneurisation
 |-|
 GitHub pour le versionnement</t>
+  </si>
+  <si>
+    <t>Ce projet industriel est centré sur l'analyse détaillée des performances d'une ligne de conditionnement automatisée. L'objectif est de déterminer précisément quels facteurs (densité, viscosité, caractéristiques physiques des produits, conditions environnementales et types d'emballage) influencent significativement la performance opérationnelle, afin de proposer des leviers d'amélioration concrets.</t>
+  </si>
+  <si>
+    <t>Identifier clairement les paramètres critiques qui affectent la cadence et la performance globale d'une ligne de conditionnement afin d'en améliorer l'efficacité opérationnelle</t>
+  </si>
+  <si>
+    <t>Comment optimiser la performance d'une ligne de conditionnement en identifiant et en contrôlant les principaux facteurs d'influence sur la cadence et la fiabilité opérationnelle ?</t>
+  </si>
+  <si>
+    <t>Développement d'un modèle prédictif pour anticiper les impacts des variations de paramètres en temps réel.
+|-|
+Intégration de scénarios plus diversifiés pour mieux anticiper les performances sous différentes conditions opérationnelles.</t>
+  </si>
+  <si>
+    <t>Identification des principaux paramètres impactant la performance (densité, viscosité, ratio produit/cadence).
+|-|
+Proposition de recommandations pratiques pour optimiser la cadence.</t>
+  </si>
+  <si>
+    <t>Les données intègrent des anomalies et des irrégularités temporelles.</t>
+  </si>
+  <si>
+    <t>Extraction et consolidation des données depuis la base SQL Server.
+|-|
+Nettoyage et prétraitement des données temporelles avec Python.
+|-|
+Développement des mesures analytiques en DAX.
+|-|
+Création du rapport interactif avec Power BI.
+|-|
+Mise en place de mesures d'amélioration</t>
+  </si>
+  <si>
+    <t>Extraction et consolidation des données depuis la base de données.
+|-|
+Nettoyage et prétraitement des données temporelles.
+|-|
+Développement des mesures analytiques en DAX.
+|-|
+Création du rapport interactif avec Power BI.
+|-|
+Mise en place de mesures d'amélioration</t>
+  </si>
+  <si>
+    <t>facteurs_influence_results.webp</t>
+  </si>
+  <si>
+    <t>facteurs_influence_data.webp</t>
+  </si>
+  <si>
+    <t>flixoucreuse_data.webp</t>
+  </si>
+  <si>
+    <t>Dans le cadre de l'analyse détaillée des performances lors de championnats sportifs, notamment en judo, l'identification, l'analyse biomécanique des techniques utilisées et l'interraction entre les athlètes constituent un réel défi. Ce projet répond au besoin de suivre précisément les mouvements des judokas afin de permettre une analyse des facteurs de placement pouvant impacter la performance globale.</t>
+  </si>
+  <si>
+    <t>Détection et suivi précis des individus avec estimation de leurs poses pour une analyse détaillée des mouvements et des interractions entre judoka.</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Obtention d'une vidéo annotée permettant de visualiser clairement les positions et les mouvements des judokas.
+|-|
+Obtention de données chiffrées de positionnement dans l'espace des corps.</t>
+  </si>
+  <si>
+    <t>Défis techniques liés à la précision de détection des poses en cas de mouvements rapides et de chevauchement.
+|-|
+Ajustement fin des paramètres du tracker (DeepSORT) pour une performance optimale
+|-|
+Récupération de données fiables des positions des corps dans l'espace 3D (surtout pour la profondeur)
+|-|
+Trouver une méthodologie de calcul pour l'intérraction entre les deux judoka.</t>
+  </si>
+  <si>
+    <t>Optimisation de la vitesse de traitement pour une analyse en temps réel améliorée.
+|-|
+Exploration de techniques avancées d'apprentissage profond pour améliorer la précision des détections.
+|-|
+Entrainnement et mise en place d'un modèle de reconnaissance de technique pour classer les interractions automatiquement</t>
   </si>
   <si>
     <t>Développement du backend avec Flask et SQLAlchemy.
@@ -743,67 +800,43 @@
 |-|
 Conteneurisation de l’application avec Docker.
 |-|
-Déploiement de l’application.</t>
-  </si>
-  <si>
-    <t>Ce projet industriel est centré sur l'analyse détaillée des performances d'une ligne de conditionnement automatisée. L'objectif est de déterminer précisément quels facteurs (densité, viscosité, caractéristiques physiques des produits, conditions environnementales et types d'emballage) influencent significativement la performance opérationnelle, afin de proposer des leviers d'amélioration concrets.</t>
-  </si>
-  <si>
-    <t>Identifier clairement les paramètres critiques qui affectent la cadence et la performance globale d'une ligne de conditionnement afin d'en améliorer l'efficacité opérationnelle</t>
-  </si>
-  <si>
-    <t>Comment optimiser la performance d'une ligne de conditionnement en identifiant et en contrôlant les principaux facteurs d'influence sur la cadence et la fiabilité opérationnelle ?</t>
-  </si>
-  <si>
-    <t>Développement d'un modèle prédictif pour anticiper les impacts des variations de paramètres en temps réel.
-|-|
-Intégration de scénarios plus diversifiés pour mieux anticiper les performances sous différentes conditions opérationnelles.</t>
-  </si>
-  <si>
-    <t>Identification des principaux paramètres impactant la performance (densité, viscosité, ratio produit/cadence).
-|-|
-Proposition de recommandations pratiques pour optimiser la cadence.</t>
-  </si>
-  <si>
-    <t>Les données intègrent des anomalies et des irrégularités temporelles.</t>
-  </si>
-  <si>
-    <t>Extraction et consolidation des données depuis la base SQL Server.
-|-|
-Nettoyage et prétraitement des données temporelles avec Python.
-|-|
-Développement des mesures analytiques en DAX.
-|-|
-Création du rapport interactif avec Power BI.
-|-|
-Mise en place de mesures d'amélioration</t>
-  </si>
-  <si>
-    <t>Extraction et consolidation des données depuis la base de données.
-|-|
-Nettoyage et prétraitement des données temporelles.
-|-|
-Développement des mesures analytiques en DAX.
-|-|
-Création du rapport interactif avec Power BI.
-|-|
-Mise en place de mesures d'amélioration</t>
-  </si>
-  <si>
-    <t>facteurs_influence_results.webp</t>
-  </si>
-  <si>
-    <t>facteurs_influence_data.webp</t>
-  </si>
-  <si>
-    <t>flixoucreuse_data.webp</t>
+Déploiement de l’application. ##on-going##</t>
+  </si>
+  <si>
+    <t>Collecte et extraction des données IMDB et TMDB.
+|-|
+Nettoyage, jointures et exploration approfondie des données.
+|-|
+Identification des caractéristiques importantes pour le modèle.
+|-|
+Développement et entraînement d'un modèle de recommandation basé sur le machine learning.
+|-|
+Création d’une interface interactive avec Streamlit pour afficher les recommandations</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>On-going</t>
+  </si>
+  <si>
+    <t>Etat_projet</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Détection et Suivi des Judokas ##done##
+|-|
+Estimation de Pose et Analyse Biomécanique ##on-going## 
+|-|
+Reconnaissance des Techniques et Séquences de Combat 
+|-|
+Traitement et Visualisation des Données</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -828,6 +861,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -877,7 +916,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -897,12 +936,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="29">
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1026,35 +1071,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA343F91-ABD2-41F5-B074-A3DB5ED79D55}" name="Tableau1" displayName="Tableau1" ref="A1:Z10" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="A1:Z10" xr:uid="{BA343F91-ABD2-41F5-B074-A3DB5ED79D55}"/>
-  <tableColumns count="26">
-    <tableColumn id="1" xr3:uid="{7E76F91B-E618-41EE-9C37-B7202AB690DD}" name="id" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{4A6F015C-59BD-48A4-9884-9E28BA1294A4}" name="title" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{01EB81F2-B04C-43B2-8D3B-3DAA19ECF415}" name="description" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{6534B8D9-E907-4BC2-8788-A60BF8C38512}" name="image_url" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{8F826BC0-97B6-48DC-B535-ADEE2F1B649E}" name="image_alt" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{574F570A-18F3-4000-BDE3-83B7EE7A33BE}" name="tags" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{699FA15F-FD6A-4B94-9225-CAAD7C6545DA}" name="description_detail" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{6BC2C552-52A7-439D-843A-68F3486D8D87}" name="objectif_projet" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{EC928EC9-7B64-496B-AF1F-E45343203EF7}" name="Probleme_resolu" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{9104D129-D3BA-4E5E-BA1E-BC76245DBC60}" name="data_source" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{8C6A8EDC-0C5F-441D-898F-EEBDF9CC02E0}" name="data_size" dataDxfId="15"/>
-    <tableColumn id="12" xr3:uid="{DB23C4AA-C25C-4F2C-BDF4-AED3372333E3}" name="data_type" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{E0842EEC-4206-4C08-91FF-7F7760EE4E81}" name="data_remark" dataDxfId="13"/>
-    <tableColumn id="14" xr3:uid="{5C91EE04-3E23-4E51-AF03-7150476816C1}" name="url_img_data" dataDxfId="12"/>
-    <tableColumn id="15" xr3:uid="{ABDDD609-BAE0-40F8-8802-E54082C0A6FA}" name="alt_img_data" dataDxfId="11"/>
-    <tableColumn id="16" xr3:uid="{4ADFAE86-3986-4940-B453-C946FFD7C9E6}" name="project_steps" dataDxfId="10"/>
-    <tableColumn id="17" xr3:uid="{49A4ADD7-02AF-4B22-B891-A75758FB681A}" name="techno" dataDxfId="9"/>
-    <tableColumn id="18" xr3:uid="{C1626FB7-43B5-48C6-94EC-6B0B88154189}" name="result" dataDxfId="8"/>
-    <tableColumn id="19" xr3:uid="{8012E277-42C6-4B8E-BE6E-679FCD796CBB}" name="img_results" dataDxfId="7"/>
-    <tableColumn id="20" xr3:uid="{23DCDF7C-22E8-49B4-A027-B8FA550C2CC8}" name="alt_img_results" dataDxfId="6"/>
-    <tableColumn id="21" xr3:uid="{AAD7C8DA-C396-4440-ABD3-1C9F99A9F70A}" name="powerbi_link" dataDxfId="5"/>
-    <tableColumn id="22" xr3:uid="{01CC34CC-A477-4637-AAEB-EA8D3B91B7B2}" name="github_link" dataDxfId="4"/>
-    <tableColumn id="23" xr3:uid="{BF856CDB-8E06-4FEF-98B3-A6B13477DC33}" name="streamlit_link" dataDxfId="3"/>
-    <tableColumn id="24" xr3:uid="{DA2CC5FB-F5D0-4B62-B17D-44C236CCCD8D}" name="video_link" dataDxfId="2"/>
-    <tableColumn id="25" xr3:uid="{B40FC4B2-4C85-474B-84F2-CCB290ABA8C2}" name="difficulties_learns" dataDxfId="1"/>
-    <tableColumn id="26" xr3:uid="{7BD0E41A-775D-478B-97C4-8EED85D35711}" name="potential_improvement" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA343F91-ABD2-41F5-B074-A3DB5ED79D55}" name="Tableau1" displayName="Tableau1" ref="A1:AA10" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+  <autoFilter ref="A1:AA10" xr:uid="{BA343F91-ABD2-41F5-B074-A3DB5ED79D55}"/>
+  <tableColumns count="27">
+    <tableColumn id="1" xr3:uid="{7E76F91B-E618-41EE-9C37-B7202AB690DD}" name="id" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{4A6F015C-59BD-48A4-9884-9E28BA1294A4}" name="title" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{01EB81F2-B04C-43B2-8D3B-3DAA19ECF415}" name="description" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{6534B8D9-E907-4BC2-8788-A60BF8C38512}" name="image_url" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{8F826BC0-97B6-48DC-B535-ADEE2F1B649E}" name="image_alt" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{574F570A-18F3-4000-BDE3-83B7EE7A33BE}" name="tags" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{699FA15F-FD6A-4B94-9225-CAAD7C6545DA}" name="description_detail" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{6BC2C552-52A7-439D-843A-68F3486D8D87}" name="objectif_projet" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{EC928EC9-7B64-496B-AF1F-E45343203EF7}" name="Probleme_resolu" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{9104D129-D3BA-4E5E-BA1E-BC76245DBC60}" name="data_source" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{8C6A8EDC-0C5F-441D-898F-EEBDF9CC02E0}" name="data_size" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{DB23C4AA-C25C-4F2C-BDF4-AED3372333E3}" name="data_type" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{E0842EEC-4206-4C08-91FF-7F7760EE4E81}" name="data_remark" dataDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{5C91EE04-3E23-4E51-AF03-7150476816C1}" name="url_img_data" dataDxfId="13"/>
+    <tableColumn id="15" xr3:uid="{ABDDD609-BAE0-40F8-8802-E54082C0A6FA}" name="alt_img_data" dataDxfId="12"/>
+    <tableColumn id="16" xr3:uid="{4ADFAE86-3986-4940-B453-C946FFD7C9E6}" name="project_steps" dataDxfId="11"/>
+    <tableColumn id="17" xr3:uid="{49A4ADD7-02AF-4B22-B891-A75758FB681A}" name="techno" dataDxfId="10"/>
+    <tableColumn id="18" xr3:uid="{C1626FB7-43B5-48C6-94EC-6B0B88154189}" name="result" dataDxfId="9"/>
+    <tableColumn id="19" xr3:uid="{8012E277-42C6-4B8E-BE6E-679FCD796CBB}" name="img_results" dataDxfId="8"/>
+    <tableColumn id="20" xr3:uid="{23DCDF7C-22E8-49B4-A027-B8FA550C2CC8}" name="alt_img_results" dataDxfId="7"/>
+    <tableColumn id="21" xr3:uid="{AAD7C8DA-C396-4440-ABD3-1C9F99A9F70A}" name="powerbi_link" dataDxfId="6"/>
+    <tableColumn id="22" xr3:uid="{01CC34CC-A477-4637-AAEB-EA8D3B91B7B2}" name="github_link" dataDxfId="5"/>
+    <tableColumn id="23" xr3:uid="{BF856CDB-8E06-4FEF-98B3-A6B13477DC33}" name="streamlit_link" dataDxfId="4"/>
+    <tableColumn id="24" xr3:uid="{DA2CC5FB-F5D0-4B62-B17D-44C236CCCD8D}" name="video_link" dataDxfId="3"/>
+    <tableColumn id="25" xr3:uid="{B40FC4B2-4C85-474B-84F2-CCB290ABA8C2}" name="difficulties_learns" dataDxfId="2"/>
+    <tableColumn id="26" xr3:uid="{7BD0E41A-775D-478B-97C4-8EED85D35711}" name="potential_improvement" dataDxfId="1"/>
+    <tableColumn id="27" xr3:uid="{59FC2E64-6C26-403A-9EE0-8346D224BD17}" name="Etat_projet" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1345,13 +1391,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z25"/>
+  <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomRight" activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1380,11 +1426,12 @@
     <col min="22" max="22" width="20" customWidth="1"/>
     <col min="23" max="24" width="17.5703125" customWidth="1"/>
     <col min="25" max="26" width="66.28515625" customWidth="1"/>
+    <col min="27" max="27" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1423,10 +1470,10 @@
         <v>66</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="P1" s="4" t="s">
         <v>67</v>
@@ -1438,10 +1485,10 @@
         <v>68</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="U1" s="3" t="s">
         <v>4</v>
@@ -1461,8 +1508,11 @@
       <c r="Z1" s="4" t="s">
         <v>71</v>
       </c>
+      <c r="AA1" s="7" t="s">
+        <v>205</v>
+      </c>
     </row>
-    <row r="2" spans="1:26" ht="240" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="240" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -1482,46 +1532,46 @@
         <v>12</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="O2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="U2" s="6" t="s">
         <v>11</v>
@@ -1530,13 +1580,16 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>203</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="225" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="225" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1556,46 +1609,46 @@
         <v>12</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="S3" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>199</v>
-      </c>
       <c r="T3" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="U3" s="2" t="s">
         <v>16</v>
@@ -1605,10 +1658,13 @@
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2" t="s">
-        <v>194</v>
+        <v>187</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>203</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="180" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1628,42 +1684,46 @@
         <v>30</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="M4" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="R4" s="5" t="s">
-        <v>81</v>
+        <v>198</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="U4" s="2"/>
       <c r="V4" s="2" t="s">
@@ -1671,16 +1731,19 @@
       </c>
       <c r="W4" s="2"/>
       <c r="X4" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="Y4" s="5" t="s">
-        <v>82</v>
+        <v>199</v>
       </c>
       <c r="Z4" s="5" t="s">
-        <v>83</v>
+        <v>200</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>204</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="345" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="345" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1700,44 +1763,44 @@
         <v>35</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="K5" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="R5" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="P5" s="2" t="s">
+      <c r="S5" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="T5" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>151</v>
       </c>
       <c r="U5" s="2"/>
       <c r="V5" s="2" t="s">
@@ -1746,13 +1809,16 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
       <c r="Y5" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="270" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="270" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -1772,36 +1838,36 @@
         <v>46</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="M6" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
@@ -1812,13 +1878,16 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
       <c r="Y6" s="2" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>203</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="315" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="360.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -1838,36 +1907,36 @@
         <v>50</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>185</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
@@ -1878,13 +1947,16 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="2" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="Z7" s="2" t="s">
-        <v>186</v>
+        <v>180</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="315" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="300" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -1904,46 +1976,46 @@
         <v>41</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="K8" s="2" t="s">
+      <c r="N8" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="R8" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="L8" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="M8" s="2" t="s">
+      <c r="S8" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="N8" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>164</v>
-      </c>
       <c r="T8" s="2" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="U8" s="2"/>
       <c r="V8" s="2" t="s">
@@ -1954,13 +2026,16 @@
       </c>
       <c r="X8" s="2"/>
       <c r="Y8" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="Z8" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
+      </c>
+      <c r="AA8" s="2" t="s">
+        <v>203</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="270" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="270" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -1980,46 +2055,46 @@
         <v>21</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="J9" s="2" t="s">
+      <c r="N9" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="R9" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="R9" s="2" t="s">
+      <c r="S9" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="T9" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="S9" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="T9" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="U9" s="2" t="s">
         <v>19</v>
@@ -2030,13 +2105,16 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
       <c r="Y9" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="Z9" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
+      </c>
+      <c r="AA9" s="2" t="s">
+        <v>203</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="360" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" ht="360" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -2056,46 +2134,46 @@
         <v>26</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="J10" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="R10" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="K10" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="R10" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="S10" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="U10" s="2" t="s">
         <v>24</v>
@@ -2106,14 +2184,17 @@
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="Z10" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
+      </c>
+      <c r="AA10" s="2" t="s">
+        <v>203</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="85.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:26" ht="85.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:27" ht="85.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:27" ht="85.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q23" s="1"/>
     </row>

</xml_diff>